<commit_message>
Added example country and modified how to choose input files and result names
</commit_message>
<xml_diff>
--- a/pyonsset2018/specs.xlsx
+++ b/pyonsset2018/specs.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -94,7 +94,7 @@
     <t>Country</t>
   </si>
   <si>
-    <t>country</t>
+    <t>Lumenia</t>
   </si>
 </sst>
 </file>
@@ -461,21 +461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -561,6 +551,39 @@
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B2">
+        <v>10000000</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>15000000</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>0.9</v>
+      </c>
+      <c r="K2">
+        <v>1.3</v>
+      </c>
+      <c r="L2">
+        <v>0.05</v>
+      </c>
+      <c r="M2">
+        <v>2000</v>
+      </c>
+      <c r="N2">
+        <v>0.2</v>
+      </c>
       <c r="O2">
         <v>0.5</v>
       </c>
@@ -570,20 +593,23 @@
       <c r="Q2">
         <v>50</v>
       </c>
+      <c r="R2">
+        <v>0.3</v>
+      </c>
       <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2">
         <v>15</v>
       </c>
-      <c r="U2">
-        <v>5</v>
-      </c>
-      <c r="V2">
-        <v>5</v>
-      </c>
       <c r="W2">
+        <v>1000</v>
+      </c>
+      <c r="X2">
         <v>3000</v>
-      </c>
-      <c r="X2">
-        <v>8000</v>
       </c>
       <c r="Y2">
         <v>10</v>

</xml_diff>